<commit_message>
Mais graficos para exp 3
</commit_message>
<xml_diff>
--- a/Exp3/Dados/buck/buck.xlsx
+++ b/Exp3/Dados/buck/buck.xlsx
@@ -40,7 +40,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -62,6 +62,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -170,7 +176,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
@@ -188,7 +194,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -218,6 +224,204 @@
             <a:ln w="28800">
               <a:solidFill>
                 <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vo teórico [V]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -265,145 +469,47 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Plan1!$B$2:$B$8</c:f>
+              <c:f>Plan1!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.44</c:v>
+                  <c:v>2.34146341463415</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.09</c:v>
+                  <c:v>5.90769230769231</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.78</c:v>
+                  <c:v>8.22857142857143</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.85</c:v>
+                  <c:v>9.54037267080745</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.5</c:v>
+                  <c:v>10.3004291845494</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>10.7663551401869</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.3</c:v>
+                  <c:v>11.0682352941176</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Plan1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Vo teórico [V]</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Plan1!$A$2:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Plan1!$C$2:$C$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="41400686"/>
-        <c:axId val="66004892"/>
+        <c:axId val="30880436"/>
+        <c:axId val="89290078"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41400686"/>
+        <c:axId val="30880436"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -432,12 +538,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66004892"/>
+        <c:crossAx val="89290078"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66004892"/>
+        <c:axId val="89290078"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,7 +558,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -481,7 +587,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41400686"/>
+        <c:crossAx val="30880436"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -529,9 +635,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>53280</xdr:colOff>
+      <xdr:colOff>52920</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>46440</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -540,7 +646,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="155160" y="1651680"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:ext cx="5774400" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -558,17 +664,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7975708502024"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8461538461538"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -594,6 +700,14 @@
         <f aca="false">12*A2/100</f>
         <v>1.2</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">12*(A2/100)*(A2/100)/((A2/100)*(A2/100) + 2*H2)</f>
+        <v>2.34146341463415</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">0.25*3*1000*0.00033/12</f>
+        <v>0.020625</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -606,6 +720,14 @@
         <f aca="false">12*A3/100</f>
         <v>2.4</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">12*(A3/100)*(A3/100)/((A3/100)*(A3/100) + 2*H3)</f>
+        <v>5.90769230769231</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">0.25*3*1000*0.00033/12</f>
+        <v>0.020625</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -618,6 +740,14 @@
         <f aca="false">12*A4/100</f>
         <v>3.6</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">12*(A4/100)*(A4/100)/((A4/100)*(A4/100) + 2*H4)</f>
+        <v>8.22857142857143</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">0.25*3*1000*0.00033/12</f>
+        <v>0.020625</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -630,6 +760,14 @@
         <f aca="false">12*A5/100</f>
         <v>4.8</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">12*(A5/100)*(A5/100)/((A5/100)*(A5/100) + 2*H5)</f>
+        <v>9.54037267080745</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">0.25*3*1000*0.00033/12</f>
+        <v>0.020625</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -642,6 +780,14 @@
         <f aca="false">12*A6/100</f>
         <v>6</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">12*(A6/100)*(A6/100)/((A6/100)*(A6/100) + 2*H6)</f>
+        <v>10.3004291845494</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">0.25*3*1000*0.00033/12</f>
+        <v>0.020625</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -654,6 +800,14 @@
         <f aca="false">12*A7/100</f>
         <v>7.2</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">12*(A7/100)*(A7/100)/((A7/100)*(A7/100) + 2*H7)</f>
+        <v>10.7663551401869</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <f aca="false">0.25*3*1000*0.00033/12</f>
+        <v>0.020625</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -665,6 +819,14 @@
       <c r="C8" s="0" t="n">
         <f aca="false">12*A8/100</f>
         <v>8.4</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">12*(A8/100)*(A8/100)/((A8/100)*(A8/100) + 2*H8)</f>
+        <v>11.0682352941176</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">0.25*3*1000*0.00033/12</f>
+        <v>0.020625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>